<commit_message>
update labels for list, and default\baseline filename; plot combined scenario
</commit_message>
<xml_diff>
--- a/scenarios_LiST_Bangladesh.xlsx
+++ b/scenarios_LiST_Bangladesh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/discworld/Documents/Research/Health/Optima/Nutrition/documentation/Countries/bangladesh/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/discworld/Documents/Research/Health/Optima/Nutrition/development/Nutrition/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="42">
   <si>
     <t>Percent of children in different height for age statuses (Stunting) (Total (0-60 months))</t>
   </si>
@@ -144,10 +144,28 @@
     <t>Total population (0-4 years) from DemProj (as opposed to 5-14 years or other categories)</t>
   </si>
   <si>
-    <t>Breastfeeding + complementary</t>
+    <t>scenario</t>
   </si>
   <si>
-    <t>scenario</t>
+    <t>CF to 30%</t>
+  </si>
+  <si>
+    <t>CF to 50%</t>
+  </si>
+  <si>
+    <t>CF to 70%</t>
+  </si>
+  <si>
+    <t>BF to 70%</t>
+  </si>
+  <si>
+    <t>BF to 80%</t>
+  </si>
+  <si>
+    <t>BF to 90%</t>
+  </si>
+  <si>
+    <t>BF to 90% + CF to 70%</t>
   </si>
 </sst>
 </file>
@@ -1315,11 +1333,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2121231552"/>
-        <c:axId val="-2121172384"/>
+        <c:axId val="2117488912"/>
+        <c:axId val="2117491792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121231552"/>
+        <c:axId val="2117488912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,7 +1347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121172384"/>
+        <c:crossAx val="2117491792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1337,7 +1355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121172384"/>
+        <c:axId val="2117491792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,7 +1366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121231552"/>
+        <c:crossAx val="2117488912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2462,11 +2480,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2111605392"/>
-        <c:axId val="-2111284896"/>
+        <c:axId val="2116902048"/>
+        <c:axId val="2116905088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111605392"/>
+        <c:axId val="2116902048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2476,7 +2494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111284896"/>
+        <c:crossAx val="2116905088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2484,7 +2502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111284896"/>
+        <c:axId val="2116905088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2513,7 +2531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111605392"/>
+        <c:crossAx val="2116902048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2961,11 +2979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2119317248"/>
-        <c:axId val="-2086985616"/>
+        <c:axId val="2114674656"/>
+        <c:axId val="2114677632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2119317248"/>
+        <c:axId val="2114674656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2975,7 +2993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2086985616"/>
+        <c:crossAx val="2114677632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2983,7 +3001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2086985616"/>
+        <c:axId val="2114677632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2994,7 +3012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119317248"/>
+        <c:crossAx val="2114674656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3425,11 +3443,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2106612768"/>
-        <c:axId val="-2108535792"/>
+        <c:axId val="2114749648"/>
+        <c:axId val="2114752624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2106612768"/>
+        <c:axId val="2114749648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3439,7 +3457,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108535792"/>
+        <c:crossAx val="2114752624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3447,7 +3465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108535792"/>
+        <c:axId val="2114752624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3458,7 +3476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106612768"/>
+        <c:crossAx val="2114749648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3889,11 +3907,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2120129264"/>
-        <c:axId val="-2106053088"/>
+        <c:axId val="2117653968"/>
+        <c:axId val="2117656944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120129264"/>
+        <c:axId val="2117653968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3903,7 +3921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106053088"/>
+        <c:crossAx val="2117656944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3911,7 +3929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2106053088"/>
+        <c:axId val="2117656944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3922,7 +3940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120129264"/>
+        <c:crossAx val="2117653968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4353,11 +4371,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2111533616"/>
-        <c:axId val="-2108117536"/>
+        <c:axId val="2117706640"/>
+        <c:axId val="2117709616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111533616"/>
+        <c:axId val="2117706640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4367,7 +4385,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108117536"/>
+        <c:crossAx val="2117709616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4375,7 +4393,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108117536"/>
+        <c:axId val="2117709616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4386,7 +4404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111533616"/>
+        <c:crossAx val="2117706640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18438,7 +18456,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18448,7 +18466,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7">
         <f>Summary!B2</f>
@@ -18586,7 +18604,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <f>Summary!B4</f>
@@ -18655,7 +18673,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <f>Summary!B5</f>
@@ -18724,7 +18742,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <f>Summary!B6</f>
@@ -18793,7 +18811,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <f>Summary!B7</f>
@@ -18862,7 +18880,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <f>Summary!B8</f>
@@ -18931,7 +18949,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <f>Summary!B9</f>
@@ -19000,7 +19018,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <f>Summary!B10</f>
@@ -19076,7 +19094,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19085,7 +19105,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7">
         <f>Summary!B2</f>
@@ -19215,7 +19235,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <f>Summary!B46</f>
@@ -19280,7 +19300,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <f>Summary!B47</f>
@@ -19345,7 +19365,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <f>Summary!B48</f>
@@ -19410,7 +19430,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <f>Summary!B49</f>
@@ -19475,7 +19495,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <f>Summary!B50</f>
@@ -19540,7 +19560,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <f>Summary!B51</f>
@@ -19605,7 +19625,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <f>Summary!B52</f>
@@ -19677,7 +19697,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19686,7 +19708,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7">
         <f>Summary!B2</f>
@@ -19816,7 +19838,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B3" s="9">
         <f>Summary!B35</f>
@@ -19881,7 +19903,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9">
         <f>Summary!B36</f>
@@ -19946,7 +19968,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9">
         <f>Summary!B37</f>
@@ -20011,7 +20033,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B6" s="9">
         <f>Summary!B38</f>
@@ -20076,7 +20098,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B7" s="9">
         <f>Summary!B39</f>
@@ -20141,7 +20163,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B8" s="9">
         <f>Summary!B40</f>
@@ -20206,7 +20228,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B9" s="9">
         <f>Summary!B41</f>

</xml_diff>